<commit_message>
bug fix scan & open fail
</commit_message>
<xml_diff>
--- a/bug/buglist.xlsx
+++ b/bug/buglist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -234,6 +234,26 @@
   <si>
     <t>sync 시에 usercode를 삭제하는데, 에러처리가 없었음.
 에러처리 추가.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>높음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부팅 후, 인증안됨.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#2 를 수정하며 생긴 사이드이펙트. Update할 내용이 없을 경우, scan을 시작하는 코드가 누락되었었습니다. (2015-01-10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -641,7 +661,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -923,15 +943,31 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
+    <row r="12" spans="1:8" ht="33">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="6">
+        <v>42012</v>
+      </c>
+      <c r="G12" s="6">
+        <v>42014</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4"/>

</xml_diff>